<commit_message>
Commit to switch branches
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_13.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_13.xlsx
@@ -54,9 +54,6 @@
     <t>Прочие долгосрочные финансовые обязательства</t>
   </si>
   <si>
-    <t xml:space="preserve">Займы полученные </t>
-  </si>
-  <si>
     <t>Долгосрочные финансовые обязательства (сумма строк 5, 6)</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>&lt;dd.MM.yyyy&gt;</t>
+  </si>
+  <si>
+    <t>Займы полученные</t>
   </si>
 </sst>
 </file>
@@ -482,6 +482,12 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
@@ -498,12 +504,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -827,7 +827,7 @@
   <dimension ref="A1:AK66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,11 +859,11 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="20"/>
@@ -887,16 +887,16 @@
       <c r="AC1" s="18"/>
       <c r="AD1" s="18"/>
       <c r="AE1" s="50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="51"/>
       <c r="E2" s="20"/>
@@ -920,7 +920,7 @@
       <c r="AC2" s="18"/>
       <c r="AD2" s="18"/>
       <c r="AE2" s="50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -948,7 +948,7 @@
       <c r="AC3" s="18"/>
       <c r="AD3" s="18"/>
       <c r="AE3" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
       <c r="AC4" s="18"/>
       <c r="AD4" s="18"/>
       <c r="AE4" s="50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -1010,7 +1010,7 @@
       <c r="AC5" s="48"/>
       <c r="AD5" s="48"/>
       <c r="AE5" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
@@ -1048,74 +1048,74 @@
       <c r="AE8" s="44"/>
     </row>
     <row r="9" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
-      <c r="X9" s="62"/>
-      <c r="Y9" s="62"/>
-      <c r="Z9" s="62"/>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="62"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="62"/>
-      <c r="AE9" s="62"/>
+      <c r="A9" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
+      <c r="V9" s="56"/>
+      <c r="W9" s="56"/>
+      <c r="X9" s="56"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="56"/>
+      <c r="AB9" s="56"/>
+      <c r="AC9" s="56"/>
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56"/>
     </row>
     <row r="10" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
-      <c r="U10" s="62"/>
-      <c r="V10" s="62"/>
-      <c r="W10" s="62"/>
-      <c r="X10" s="62"/>
-      <c r="Y10" s="62"/>
-      <c r="Z10" s="62"/>
-      <c r="AA10" s="62"/>
-      <c r="AB10" s="62"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="62"/>
-      <c r="AE10" s="62"/>
+      <c r="A10" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="56"/>
+      <c r="V10" s="56"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="56"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="56"/>
+      <c r="AB10" s="56"/>
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B11" s="43"/>
@@ -1156,138 +1156,138 @@
       <c r="AC12" s="42"/>
     </row>
     <row r="13" spans="1:32" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="63" t="s">
+      <c r="A13" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="B13" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="C13" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="D13" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="63" t="s">
+      <c r="E13" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="63" t="s">
+      <c r="F13" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="63" t="s">
+      <c r="G13" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="H13" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="58" t="s">
+      <c r="I13" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="59"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="58" t="s">
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="59"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59"/>
-      <c r="AC13" s="59"/>
-      <c r="AD13" s="59"/>
-      <c r="AE13" s="60"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="61"/>
+      <c r="T13" s="61"/>
+      <c r="U13" s="61"/>
+      <c r="V13" s="61"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="61"/>
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="61"/>
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="61"/>
+      <c r="AE13" s="62"/>
       <c r="AF13" s="41"/>
     </row>
     <row r="14" spans="1:32" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
       <c r="I14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="Q14" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="R14" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="31" t="s">
+      <c r="S14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="31" t="s">
+      <c r="T14" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="31" t="s">
+      <c r="U14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="31" t="s">
+      <c r="V14" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="P14" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q14" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="R14" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="S14" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="T14" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="U14" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="V14" s="31" t="s">
-        <v>20</v>
-      </c>
       <c r="W14" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="X14" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Y14" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z14" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA14" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB14" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AC14" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD14" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AE14" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AF14" s="20"/>
     </row>
@@ -1390,7 +1390,7 @@
     <row r="16" spans="1:32" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="28">
         <v>1</v>
@@ -1428,7 +1428,7 @@
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C17" s="31">
         <v>2</v>
@@ -1466,7 +1466,7 @@
     <row r="18" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="27">
         <v>3</v>
@@ -1506,7 +1506,7 @@
     <row r="19" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="33">
         <v>4</v>
@@ -1546,7 +1546,7 @@
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
       <c r="B20" s="32" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C20" s="31">
         <v>5</v>
@@ -1624,10 +1624,10 @@
       <c r="AH21" s="20"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="61"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="28">
         <v>7</v>
       </c>
@@ -1703,179 +1703,179 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
-      <c r="Q24" s="57"/>
-      <c r="R24" s="57"/>
-      <c r="S24" s="57"/>
-      <c r="T24" s="57"/>
-      <c r="U24" s="57"/>
-      <c r="V24" s="57"/>
-      <c r="W24" s="57"/>
-      <c r="X24" s="57"/>
-      <c r="Y24" s="57"/>
-      <c r="Z24" s="57"/>
-      <c r="AA24" s="57"/>
-      <c r="AB24" s="57"/>
-      <c r="AC24" s="57"/>
-      <c r="AD24" s="57"/>
-      <c r="AE24" s="57"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="59"/>
+      <c r="T24" s="59"/>
+      <c r="U24" s="59"/>
+      <c r="V24" s="59"/>
+      <c r="W24" s="59"/>
+      <c r="X24" s="59"/>
+      <c r="Y24" s="59"/>
+      <c r="Z24" s="59"/>
+      <c r="AA24" s="59"/>
+      <c r="AB24" s="59"/>
+      <c r="AC24" s="59"/>
+      <c r="AD24" s="59"/>
+      <c r="AE24" s="59"/>
       <c r="AF24" s="20"/>
       <c r="AG24" s="20"/>
       <c r="AH24" s="20"/>
     </row>
     <row r="25" spans="1:34" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="57"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="57"/>
-      <c r="U25" s="57"/>
-      <c r="V25" s="57"/>
-      <c r="W25" s="57"/>
-      <c r="X25" s="57"/>
-      <c r="Y25" s="57"/>
-      <c r="Z25" s="57"/>
-      <c r="AA25" s="57"/>
-      <c r="AB25" s="57"/>
-      <c r="AC25" s="57"/>
-      <c r="AD25" s="57"/>
-      <c r="AE25" s="57"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="59"/>
+      <c r="Y25" s="59"/>
+      <c r="Z25" s="59"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="59"/>
+      <c r="AC25" s="59"/>
+      <c r="AD25" s="59"/>
+      <c r="AE25" s="59"/>
     </row>
     <row r="26" spans="1:34" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="57"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="57"/>
-      <c r="V26" s="57"/>
-      <c r="W26" s="57"/>
-      <c r="X26" s="57"/>
-      <c r="Y26" s="57"/>
-      <c r="Z26" s="57"/>
-      <c r="AA26" s="57"/>
-      <c r="AB26" s="57"/>
-      <c r="AC26" s="57"/>
-      <c r="AD26" s="57"/>
-      <c r="AE26" s="57"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="59"/>
+      <c r="Y26" s="59"/>
+      <c r="Z26" s="59"/>
+      <c r="AA26" s="59"/>
+      <c r="AB26" s="59"/>
+      <c r="AC26" s="59"/>
+      <c r="AD26" s="59"/>
+      <c r="AE26" s="59"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="57"/>
-      <c r="P27" s="57"/>
-      <c r="Q27" s="57"/>
-      <c r="R27" s="57"/>
-      <c r="S27" s="57"/>
-      <c r="T27" s="57"/>
-      <c r="U27" s="57"/>
-      <c r="V27" s="57"/>
-      <c r="W27" s="57"/>
-      <c r="X27" s="57"/>
-      <c r="Y27" s="57"/>
-      <c r="Z27" s="57"/>
-      <c r="AA27" s="57"/>
-      <c r="AB27" s="57"/>
-      <c r="AC27" s="57"/>
-      <c r="AD27" s="57"/>
-      <c r="AE27" s="57"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="59"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="59"/>
+      <c r="W27" s="59"/>
+      <c r="X27" s="59"/>
+      <c r="Y27" s="59"/>
+      <c r="Z27" s="59"/>
+      <c r="AA27" s="59"/>
+      <c r="AB27" s="59"/>
+      <c r="AC27" s="59"/>
+      <c r="AD27" s="59"/>
+      <c r="AE27" s="59"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="57"/>
-      <c r="U28" s="57"/>
-      <c r="V28" s="57"/>
-      <c r="W28" s="57"/>
-      <c r="X28" s="57"/>
-      <c r="Y28" s="57"/>
-      <c r="Z28" s="57"/>
-      <c r="AA28" s="57"/>
-      <c r="AB28" s="57"/>
-      <c r="AC28" s="57"/>
-      <c r="AD28" s="57"/>
-      <c r="AE28" s="57"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="59"/>
+      <c r="T28" s="59"/>
+      <c r="U28" s="59"/>
+      <c r="V28" s="59"/>
+      <c r="W28" s="59"/>
+      <c r="X28" s="59"/>
+      <c r="Y28" s="59"/>
+      <c r="Z28" s="59"/>
+      <c r="AA28" s="59"/>
+      <c r="AB28" s="59"/>
+      <c r="AC28" s="59"/>
+      <c r="AD28" s="59"/>
+      <c r="AE28" s="59"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
@@ -2985,6 +2985,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B26:AE26"/>
+    <mergeCell ref="B27:AE27"/>
+    <mergeCell ref="B28:AE28"/>
+    <mergeCell ref="I13:P13"/>
+    <mergeCell ref="Q13:W13"/>
+    <mergeCell ref="X13:AE13"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="B24:AE24"/>
+    <mergeCell ref="B25:AE25"/>
     <mergeCell ref="A9:AE9"/>
     <mergeCell ref="A10:AE10"/>
     <mergeCell ref="A13:A14"/>
@@ -2995,15 +3004,6 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
-    <mergeCell ref="B26:AE26"/>
-    <mergeCell ref="B27:AE27"/>
-    <mergeCell ref="B28:AE28"/>
-    <mergeCell ref="I13:P13"/>
-    <mergeCell ref="Q13:W13"/>
-    <mergeCell ref="X13:AE13"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="B24:AE24"/>
-    <mergeCell ref="B25:AE25"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
NICK MF Reporting: - xlsx templates corrected
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_13.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_13.xlsx
@@ -15,10 +15,10 @@
     <sheet name="РФО_13" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Database" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="GR_CODE_ROW">4583</definedName>
     <definedName name="GR_CODE_SHEET">4</definedName>
-    <definedName name="_xlnm.Database" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">РФО_13!$A$1:$AF$24</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Прочие долгосрочные финансовые обязательства</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>Итого (гр.11+гр.12+гр.13+гр.14+гр.15+гр.16)</t>
-  </si>
-  <si>
-    <t>Вознаргаждение</t>
   </si>
   <si>
     <t>Количество (гр.10+гр.18)</t>
@@ -192,7 +189,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
   </numFmts>
@@ -498,6 +495,9 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -528,14 +528,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный_ФормОтчет" xfId="2"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -852,8 +849,8 @@
   </sheetPr>
   <dimension ref="A1:AL62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,76 +1072,76 @@
       <c r="AF8" s="21"/>
     </row>
     <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="46"/>
-      <c r="W9" s="46"/>
-      <c r="X9" s="46"/>
-      <c r="Y9" s="46"/>
-      <c r="Z9" s="46"/>
-      <c r="AA9" s="46"/>
-      <c r="AB9" s="46"/>
-      <c r="AC9" s="46"/>
-      <c r="AD9" s="46"/>
-      <c r="AE9" s="46"/>
-      <c r="AF9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="47"/>
+      <c r="X9" s="47"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="47"/>
+      <c r="AA9" s="47"/>
+      <c r="AB9" s="47"/>
+      <c r="AC9" s="47"/>
+      <c r="AD9" s="47"/>
+      <c r="AE9" s="47"/>
+      <c r="AF9" s="47"/>
     </row>
     <row r="10" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="46"/>
-      <c r="W10" s="46"/>
-      <c r="X10" s="46"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="46"/>
-      <c r="AB10" s="46"/>
-      <c r="AC10" s="46"/>
-      <c r="AD10" s="46"/>
-      <c r="AE10" s="46"/>
-      <c r="AF10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="47"/>
+      <c r="AB10" s="47"/>
+      <c r="AC10" s="47"/>
+      <c r="AD10" s="47"/>
+      <c r="AE10" s="47"/>
+      <c r="AF10" s="47"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" s="20"/>
@@ -1186,74 +1183,74 @@
       <c r="AD12" s="19"/>
     </row>
     <row r="13" spans="1:33" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="49" t="s">
+      <c r="H13" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="49" t="s">
+      <c r="I13" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="51" t="s">
+      <c r="J13" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="51" t="s">
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="S13" s="52"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
-      <c r="V13" s="52"/>
-      <c r="W13" s="52"/>
-      <c r="X13" s="53"/>
-      <c r="Y13" s="51" t="s">
+      <c r="S13" s="53"/>
+      <c r="T13" s="53"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="53"/>
+      <c r="W13" s="53"/>
+      <c r="X13" s="54"/>
+      <c r="Y13" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="Z13" s="52"/>
-      <c r="AA13" s="52"/>
-      <c r="AB13" s="52"/>
-      <c r="AC13" s="52"/>
-      <c r="AD13" s="52"/>
-      <c r="AE13" s="52"/>
-      <c r="AF13" s="53"/>
+      <c r="Z13" s="53"/>
+      <c r="AA13" s="53"/>
+      <c r="AB13" s="53"/>
+      <c r="AC13" s="53"/>
+      <c r="AD13" s="53"/>
+      <c r="AE13" s="53"/>
+      <c r="AF13" s="54"/>
       <c r="AG13" s="18"/>
     </row>
     <row r="14" spans="1:33" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="31" t="s">
         <v>10</v>
       </c>
@@ -1291,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="V14" s="31" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="W14" s="31" t="s">
         <v>5</v>
@@ -1300,28 +1297,28 @@
         <v>4</v>
       </c>
       <c r="Y14" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z14" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="Z14" s="31" t="s">
+      <c r="AA14" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="AA14" s="31" t="s">
+      <c r="AB14" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="AB14" s="31" t="s">
+      <c r="AC14" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="AC14" s="31" t="s">
+      <c r="AD14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="AD14" s="31" t="s">
+      <c r="AE14" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="AE14" s="31" t="s">
+      <c r="AF14" s="31" t="s">
         <v>43</v>
-      </c>
-      <c r="AF14" s="31" t="s">
-        <v>44</v>
       </c>
       <c r="AG14" s="16"/>
     </row>
@@ -1435,7 +1432,7 @@
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
-      <c r="G16" s="54"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
       <c r="J16" s="37"/>
@@ -1466,7 +1463,7 @@
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="32">
         <v>2</v>
@@ -1554,7 +1551,7 @@
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
       <c r="F19" s="37"/>
-      <c r="G19" s="54"/>
+      <c r="G19" s="44"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
       <c r="J19" s="37"/>
@@ -1587,7 +1584,7 @@
     <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="32">
         <v>5</v>
@@ -1667,17 +1664,17 @@
       <c r="AI21" s="16"/>
     </row>
     <row r="22" spans="1:35" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="45"/>
+      <c r="A22" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="46"/>
       <c r="C22" s="36">
         <v>7</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
       <c r="F22" s="37"/>
-      <c r="G22" s="54"/>
+      <c r="G22" s="44"/>
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
       <c r="J22" s="37"/>
@@ -1740,7 +1737,7 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
@@ -1776,7 +1773,7 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
@@ -1812,7 +1809,7 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -1848,7 +1845,7 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
@@ -1884,7 +1881,7 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>

</xml_diff>